<commit_message>
update generate_teacher_load in report_module.py file
</commit_message>
<xml_diff>
--- a/teacher_load.xlsx
+++ b/teacher_load.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>TeacherID</t>
+          <t>Teacher ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Subject Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Number of Classes</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Number of Students</t>
         </is>
       </c>
     </row>
@@ -464,11 +464,13 @@
           <t>Mr. Adams</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Math</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -480,11 +482,13 @@
           <t>Ms. Baker</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Science</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>